<commit_message>
updated the wave 3 excel sheet
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave3.xlsx
+++ b/docs/Language Waves/wave3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration feb 17\OVWMigration\docs\Language Waves\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ovwfeb19\OVWMigration\docs\Language Waves\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19410" windowHeight="7755" firstSheet="15" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="7755" firstSheet="12" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="az_az" sheetId="20" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="el_gr" sheetId="8" r:id="rId16"/>
     <sheet name="en_hk" sheetId="10" r:id="rId17"/>
     <sheet name="hu_hu" sheetId="11" r:id="rId18"/>
-    <sheet name="bg-bg" sheetId="16" r:id="rId19"/>
+    <sheet name="bg_bg" sheetId="16" r:id="rId19"/>
     <sheet name="fr_ca" sheetId="17" r:id="rId20"/>
     <sheet name="en_ca" sheetId="18" r:id="rId21"/>
     <sheet name="ro_ro" sheetId="12" r:id="rId22"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="467">
   <si>
     <t>http://www.cisco.com/web/BG/ordering/index.html</t>
   </si>
@@ -423,9 +423,6 @@
     <t>http://www.cisco.com/web/CA/products/wireless_comparison_fr.html</t>
   </si>
   <si>
-    <t>buyersguide-var2</t>
-  </si>
-  <si>
     <t>http://www.cisco.com/web/CA/products/security/index_fr.html</t>
   </si>
   <si>
@@ -795,9 +792,6 @@
     <t>http://www.cisco.com/web/ordering/root/index.html</t>
   </si>
   <si>
-    <t>http://www.cisco.com/cisco/web/support/index.html</t>
-  </si>
-  <si>
     <t>http://www.cisco.com/web/learning/index.html</t>
   </si>
   <si>
@@ -1149,9 +1143,6 @@
     <t>http://www.cisco.com/web/RO/ordering/ordering_home.html</t>
   </si>
   <si>
-    <t>http://www.cisco.com/web/RO/techsupport/techsupport_home.html</t>
-  </si>
-  <si>
     <t>http://www.cisco.com/web/RO/learn_events/index.html</t>
   </si>
   <si>
@@ -1453,6 +1444,12 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/RO/solutions/index.html</t>
+  </si>
+  <si>
+    <t>index-buyersguidevar3</t>
+  </si>
+  <si>
+    <t>buyers-guide-var2</t>
   </si>
 </sst>
 </file>
@@ -2008,7 +2005,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -2022,7 +2019,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2036,7 +2033,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -2047,7 +2044,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2058,7 +2055,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -2090,7 +2087,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2101,7 +2098,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2115,7 +2112,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2126,7 +2123,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -2137,7 +2134,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -2148,7 +2145,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2162,7 +2159,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -2176,7 +2173,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
@@ -2193,7 +2190,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -2210,7 +2207,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -2227,7 +2224,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -2244,7 +2241,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -2261,7 +2258,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -2278,7 +2275,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
@@ -2292,7 +2289,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -2309,7 +2306,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -2326,7 +2323,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
@@ -2343,7 +2340,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B18" t="s">
         <v>79</v>
@@ -2360,7 +2357,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B19" t="s">
         <v>79</v>
@@ -2377,7 +2374,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
@@ -2391,7 +2388,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -2405,7 +2402,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -2419,7 +2416,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B23" t="s">
         <v>113</v>
@@ -2436,7 +2433,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B24" t="s">
         <v>113</v>
@@ -2453,7 +2450,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B25" t="s">
         <v>118</v>
@@ -2470,7 +2467,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
@@ -2487,7 +2484,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B27" t="s">
         <v>121</v>
@@ -2504,7 +2501,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B28" t="s">
         <v>121</v>
@@ -2521,13 +2518,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
         <v>126</v>
-      </c>
-      <c r="C29" t="s">
-        <v>127</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
@@ -2538,13 +2535,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" t="s">
         <v>19</v>
@@ -2555,10 +2552,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>114</v>
@@ -2572,10 +2569,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" t="s">
         <v>116</v>
@@ -2589,13 +2586,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" t="s">
         <v>142</v>
-      </c>
-      <c r="C33" t="s">
-        <v>143</v>
       </c>
       <c r="D33" t="s">
         <v>19</v>
@@ -2606,10 +2603,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
         <v>114</v>
@@ -2623,10 +2620,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
         <v>116</v>
@@ -2640,13 +2637,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
         <v>159</v>
-      </c>
-      <c r="C36" t="s">
-        <v>160</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -2657,13 +2654,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
@@ -2674,13 +2671,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
         <v>162</v>
-      </c>
-      <c r="C38" t="s">
-        <v>163</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
@@ -2691,13 +2688,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
@@ -2708,13 +2705,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
@@ -2725,13 +2722,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
@@ -2742,13 +2739,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
         <v>19</v>
@@ -2759,13 +2756,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
         <v>19</v>
@@ -2776,13 +2773,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" t="s">
         <v>166</v>
-      </c>
-      <c r="C44" t="s">
-        <v>167</v>
       </c>
       <c r="D44" t="s">
         <v>19</v>
@@ -2793,13 +2790,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
         <v>19</v>
@@ -2810,13 +2807,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
         <v>19</v>
@@ -2827,13 +2824,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -2855,7 +2852,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,7 +2866,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2880,7 +2877,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2894,7 +2891,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -2916,7 +2913,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -2927,7 +2924,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2941,7 +2938,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -2955,7 +2952,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
@@ -2972,7 +2969,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -2989,7 +2986,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -3006,7 +3003,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -3023,7 +3020,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -3040,7 +3037,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -3057,7 +3054,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
@@ -3071,7 +3068,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -3088,7 +3085,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -3105,13 +3102,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>465</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -3122,7 +3119,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B18" t="s">
         <v>79</v>
@@ -3139,7 +3136,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B19" t="s">
         <v>79</v>
@@ -3156,7 +3153,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
@@ -3170,7 +3167,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -3184,7 +3181,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -3198,7 +3195,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B23" t="s">
         <v>113</v>
@@ -3215,7 +3212,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B24" t="s">
         <v>113</v>
@@ -3232,7 +3229,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B25" t="s">
         <v>118</v>
@@ -3249,7 +3246,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
@@ -3266,7 +3263,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B27" t="s">
         <v>121</v>
@@ -3283,7 +3280,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B28" t="s">
         <v>121</v>
@@ -3300,13 +3297,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
         <v>126</v>
-      </c>
-      <c r="C29" t="s">
-        <v>127</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
@@ -3317,13 +3314,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" t="s">
         <v>19</v>
@@ -3334,10 +3331,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>114</v>
@@ -3351,10 +3348,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" t="s">
         <v>116</v>
@@ -3368,13 +3365,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" t="s">
         <v>142</v>
-      </c>
-      <c r="C33" t="s">
-        <v>143</v>
       </c>
       <c r="D33" t="s">
         <v>19</v>
@@ -3385,10 +3382,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
         <v>114</v>
@@ -3402,10 +3399,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
         <v>116</v>
@@ -3419,13 +3416,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
         <v>159</v>
-      </c>
-      <c r="C36" t="s">
-        <v>160</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -3436,13 +3433,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
@@ -3453,13 +3450,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
         <v>162</v>
-      </c>
-      <c r="C38" t="s">
-        <v>163</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
@@ -3470,13 +3467,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
@@ -3487,13 +3484,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
@@ -3504,13 +3501,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
@@ -3521,13 +3518,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
         <v>19</v>
@@ -3538,13 +3535,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
         <v>19</v>
@@ -3555,13 +3552,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" t="s">
         <v>166</v>
-      </c>
-      <c r="C44" t="s">
-        <v>167</v>
       </c>
       <c r="D44" t="s">
         <v>19</v>
@@ -3572,13 +3569,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
         <v>19</v>
@@ -3589,13 +3586,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
         <v>19</v>
@@ -3606,13 +3603,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -3645,7 +3642,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3656,7 +3653,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -3670,7 +3667,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -3681,7 +3678,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -3692,7 +3689,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -3706,7 +3703,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -3723,7 +3720,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -3740,7 +3737,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -3776,7 +3773,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3787,7 +3784,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -3801,7 +3798,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -3812,7 +3809,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -3823,7 +3820,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -3837,7 +3834,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -3854,7 +3851,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -3871,7 +3868,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -3905,7 +3902,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3916,7 +3913,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -3930,7 +3927,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -3941,7 +3938,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -3952,7 +3949,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -3969,7 +3966,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -3986,7 +3983,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -4000,7 +3997,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -4034,7 +4031,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4045,7 +4042,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -4059,7 +4056,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -4070,7 +4067,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4081,7 +4078,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -4098,7 +4095,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -4115,7 +4112,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -4129,7 +4126,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -4162,7 +4159,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4173,7 +4170,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -4187,7 +4184,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -4198,7 +4195,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4209,7 +4206,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -4226,7 +4223,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -4243,7 +4240,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -4257,7 +4254,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -4278,8 +4275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,7 +4288,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4302,7 +4299,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -4316,7 +4313,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -4327,7 +4324,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -4338,7 +4335,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4349,7 +4346,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -4363,7 +4360,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -4377,7 +4374,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
@@ -4394,7 +4391,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -4411,7 +4408,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -4428,7 +4425,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -4445,7 +4442,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -4462,7 +4459,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -4479,7 +4476,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
@@ -4493,7 +4490,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -4510,7 +4507,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -4527,13 +4524,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>465</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -4544,7 +4541,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B18" t="s">
         <v>79</v>
@@ -4561,7 +4558,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B19" t="s">
         <v>79</v>
@@ -4578,7 +4575,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
@@ -4592,7 +4589,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -4606,7 +4603,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -4620,7 +4617,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B23" t="s">
         <v>113</v>
@@ -4637,7 +4634,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B24" t="s">
         <v>113</v>
@@ -4654,7 +4651,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B25" t="s">
         <v>118</v>
@@ -4671,7 +4668,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
@@ -4688,7 +4685,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B27" t="s">
         <v>121</v>
@@ -4705,7 +4702,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B28" t="s">
         <v>121</v>
@@ -4722,13 +4719,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
         <v>126</v>
-      </c>
-      <c r="C29" t="s">
-        <v>127</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
@@ -4739,13 +4736,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" t="s">
         <v>19</v>
@@ -4756,10 +4753,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>114</v>
@@ -4773,10 +4770,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" t="s">
         <v>116</v>
@@ -4790,13 +4787,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" t="s">
         <v>142</v>
-      </c>
-      <c r="C33" t="s">
-        <v>143</v>
       </c>
       <c r="D33" t="s">
         <v>19</v>
@@ -4807,10 +4804,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
         <v>114</v>
@@ -4824,10 +4821,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
         <v>116</v>
@@ -4841,13 +4838,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
         <v>159</v>
-      </c>
-      <c r="C36" t="s">
-        <v>160</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -4858,13 +4855,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
@@ -4875,13 +4872,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
         <v>162</v>
-      </c>
-      <c r="C38" t="s">
-        <v>163</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
@@ -4892,13 +4889,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
@@ -4909,13 +4906,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
@@ -4926,13 +4923,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
@@ -4943,13 +4940,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
         <v>19</v>
@@ -4960,13 +4957,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
         <v>19</v>
@@ -4977,13 +4974,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" t="s">
         <v>166</v>
-      </c>
-      <c r="C44" t="s">
-        <v>167</v>
       </c>
       <c r="D44" t="s">
         <v>19</v>
@@ -4994,13 +4991,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
         <v>19</v>
@@ -5011,13 +5008,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
         <v>19</v>
@@ -5028,13 +5025,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -5064,7 +5061,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -5075,7 +5072,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -5089,7 +5086,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -5100,7 +5097,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5111,7 +5108,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -5128,7 +5125,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -5145,7 +5142,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -5159,7 +5156,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -5351,7 +5348,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -5365,7 +5362,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -5379,7 +5376,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -5390,7 +5387,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -5401,7 +5398,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5419,8 +5416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5930,7 +5927,7 @@
         <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>465</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -6313,7 +6310,7 @@
         <v>121</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>466</v>
       </c>
       <c r="D55" t="s">
         <v>19</v>
@@ -6324,13 +6321,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" t="s">
         <v>125</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>126</v>
-      </c>
-      <c r="C56" t="s">
-        <v>127</v>
       </c>
       <c r="D56" t="s">
         <v>19</v>
@@ -6341,13 +6338,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" t="s">
         <v>128</v>
-      </c>
-      <c r="B57" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" t="s">
-        <v>129</v>
       </c>
       <c r="D57" t="s">
         <v>19</v>
@@ -6358,13 +6355,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" t="s">
         <v>130</v>
-      </c>
-      <c r="B58" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" t="s">
-        <v>131</v>
       </c>
       <c r="D58" t="s">
         <v>19</v>
@@ -6375,13 +6372,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" t="s">
         <v>132</v>
-      </c>
-      <c r="B59" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" t="s">
-        <v>133</v>
       </c>
       <c r="D59" t="s">
         <v>19</v>
@@ -6392,13 +6389,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" t="s">
         <v>134</v>
-      </c>
-      <c r="B60" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" t="s">
-        <v>135</v>
       </c>
       <c r="D60" t="s">
         <v>19</v>
@@ -6409,13 +6406,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" t="s">
         <v>136</v>
-      </c>
-      <c r="B61" t="s">
-        <v>126</v>
-      </c>
-      <c r="C61" t="s">
-        <v>137</v>
       </c>
       <c r="D61" t="s">
         <v>19</v>
@@ -6426,10 +6423,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" t="s">
         <v>138</v>
-      </c>
-      <c r="B62" t="s">
-        <v>139</v>
       </c>
       <c r="C62" t="s">
         <v>114</v>
@@ -6443,10 +6440,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
         <v>116</v>
@@ -6460,13 +6457,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" t="s">
         <v>141</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>142</v>
-      </c>
-      <c r="C64" t="s">
-        <v>143</v>
       </c>
       <c r="D64" t="s">
         <v>19</v>
@@ -6477,10 +6474,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" t="s">
         <v>144</v>
-      </c>
-      <c r="B65" t="s">
-        <v>145</v>
       </c>
       <c r="C65" t="s">
         <v>114</v>
@@ -6494,10 +6491,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
         <v>116</v>
@@ -6511,13 +6508,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" t="s">
         <v>159</v>
-      </c>
-      <c r="C67" t="s">
-        <v>160</v>
       </c>
       <c r="D67" t="s">
         <v>19</v>
@@ -6528,13 +6525,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" t="s">
         <v>19</v>
@@ -6545,13 +6542,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B69" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" t="s">
         <v>162</v>
-      </c>
-      <c r="C69" t="s">
-        <v>163</v>
       </c>
       <c r="D69" t="s">
         <v>19</v>
@@ -6562,13 +6559,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D70" t="s">
         <v>19</v>
@@ -6579,13 +6576,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D71" t="s">
         <v>19</v>
@@ -6596,13 +6593,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D72" t="s">
         <v>19</v>
@@ -6613,13 +6610,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D73" t="s">
         <v>19</v>
@@ -6630,13 +6627,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D74" t="s">
         <v>19</v>
@@ -6647,13 +6644,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B75" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" t="s">
         <v>166</v>
-      </c>
-      <c r="C75" t="s">
-        <v>167</v>
       </c>
       <c r="D75" t="s">
         <v>19</v>
@@ -6664,13 +6661,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D76" t="s">
         <v>19</v>
@@ -6681,13 +6678,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D77" t="s">
         <v>19</v>
@@ -6698,13 +6695,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D78" t="s">
         <v>19</v>
@@ -6715,13 +6712,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>95</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>12</v>
@@ -6800,8 +6797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6814,7 +6811,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -6825,7 +6822,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -6839,7 +6836,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -6850,7 +6847,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -6861,7 +6858,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -6872,7 +6869,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -6886,7 +6883,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -6900,7 +6897,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -6934,7 +6931,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -6951,7 +6948,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -6968,7 +6965,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -6985,7 +6982,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
@@ -7002,7 +6999,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
@@ -7019,7 +7016,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
@@ -7036,7 +7033,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s">
         <v>41</v>
@@ -7053,13 +7050,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" t="s">
         <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -7070,7 +7067,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
@@ -7087,7 +7084,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
@@ -7104,7 +7101,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
@@ -7121,7 +7118,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
@@ -7138,7 +7135,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
@@ -7155,13 +7152,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -7172,7 +7169,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
@@ -7189,7 +7186,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
@@ -7206,7 +7203,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
@@ -7223,7 +7220,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
@@ -7240,7 +7237,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
@@ -7257,7 +7254,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
         <v>71</v>
@@ -7271,7 +7268,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
@@ -7288,7 +7285,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -7305,13 +7302,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
         <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>465</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -7322,7 +7319,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
         <v>79</v>
@@ -7339,7 +7336,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B34" t="s">
         <v>79</v>
@@ -7356,7 +7353,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35" t="s">
         <v>79</v>
@@ -7373,7 +7370,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B36" t="s">
         <v>79</v>
@@ -7390,10 +7387,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D37" t="s">
         <v>91</v>
@@ -7404,7 +7401,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
         <v>93</v>
@@ -7418,7 +7415,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B39" t="s">
         <v>95</v>
@@ -7435,7 +7432,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" t="s">
         <v>95</v>
@@ -7452,7 +7449,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B41" t="s">
         <v>95</v>
@@ -7469,7 +7466,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B42" t="s">
         <v>102</v>
@@ -7486,7 +7483,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B43" t="s">
         <v>104</v>
@@ -7503,7 +7500,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B44" t="s">
         <v>104</v>
@@ -7520,7 +7517,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B45" t="s">
         <v>104</v>
@@ -7537,7 +7534,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B46" t="s">
         <v>104</v>
@@ -7554,7 +7551,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C47" t="s">
         <v>18</v>
@@ -7568,7 +7565,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
         <v>113</v>
@@ -7585,7 +7582,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B49" t="s">
         <v>113</v>
@@ -7602,7 +7599,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
         <v>118</v>
@@ -7619,7 +7616,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
         <v>118</v>
@@ -7636,7 +7633,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s">
         <v>121</v>
@@ -7653,7 +7650,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B53" t="s">
         <v>121</v>
@@ -7670,13 +7667,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B54" t="s">
         <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>466</v>
       </c>
       <c r="D54" t="s">
         <v>19</v>
@@ -7687,13 +7684,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" t="s">
         <v>126</v>
-      </c>
-      <c r="C55" t="s">
-        <v>127</v>
       </c>
       <c r="D55" t="s">
         <v>19</v>
@@ -7704,13 +7701,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
         <v>19</v>
@@ -7721,13 +7718,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D57" t="s">
         <v>19</v>
@@ -7738,13 +7735,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
         <v>19</v>
@@ -7755,13 +7752,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D59" t="s">
         <v>19</v>
@@ -7772,13 +7769,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D60" t="s">
         <v>19</v>
@@ -7789,10 +7786,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C61" t="s">
         <v>114</v>
@@ -7806,10 +7803,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C62" t="s">
         <v>116</v>
@@ -7823,13 +7820,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B63" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" t="s">
         <v>142</v>
-      </c>
-      <c r="C63" t="s">
-        <v>143</v>
       </c>
       <c r="D63" t="s">
         <v>19</v>
@@ -7840,10 +7837,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
         <v>114</v>
@@ -7857,10 +7854,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
         <v>116</v>
@@ -7874,13 +7871,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B66" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" t="s">
         <v>159</v>
-      </c>
-      <c r="C66" t="s">
-        <v>160</v>
       </c>
       <c r="D66" t="s">
         <v>19</v>
@@ -7891,13 +7888,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D67" t="s">
         <v>19</v>
@@ -7908,13 +7905,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" t="s">
         <v>162</v>
-      </c>
-      <c r="C68" t="s">
-        <v>163</v>
       </c>
       <c r="D68" t="s">
         <v>19</v>
@@ -7925,13 +7922,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" t="s">
         <v>19</v>
@@ -7942,13 +7939,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D70" t="s">
         <v>19</v>
@@ -7959,13 +7956,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D71" t="s">
         <v>19</v>
@@ -7976,13 +7973,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D72" t="s">
         <v>19</v>
@@ -7993,13 +7990,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D73" t="s">
         <v>19</v>
@@ -8010,13 +8007,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" t="s">
         <v>166</v>
-      </c>
-      <c r="C74" t="s">
-        <v>167</v>
       </c>
       <c r="D74" t="s">
         <v>19</v>
@@ -8027,13 +8024,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D75" t="s">
         <v>19</v>
@@ -8044,13 +8041,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D76" t="s">
         <v>19</v>
@@ -8061,13 +8058,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D77" t="s">
         <v>19</v>
@@ -8078,7 +8075,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>79</v>
@@ -8095,13 +8092,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>95</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>12</v>
@@ -8122,17 +8119,17 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="64.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
@@ -8140,10 +8137,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -8154,64 +8151,64 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -8222,64 +8219,43 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+        <v>368</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>253</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>371</v>
+        <v>464</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
-    <hyperlink ref="A1" r:id="rId6"/>
-    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A1" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8300,7 +8276,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -8311,7 +8287,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8325,7 +8301,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -8336,7 +8312,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -8347,7 +8323,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -8361,7 +8337,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -8378,7 +8354,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -8395,7 +8371,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -8428,7 +8404,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -8439,7 +8415,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8453,7 +8429,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -8464,7 +8440,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -8475,7 +8451,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -8489,7 +8465,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -8506,7 +8482,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -8523,7 +8499,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -8558,7 +8534,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -8569,7 +8545,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8583,7 +8559,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -8594,7 +8570,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -8605,7 +8581,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -8619,7 +8595,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -8636,7 +8612,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -8653,7 +8629,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -8687,7 +8663,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -8698,7 +8674,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8712,7 +8688,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -8723,7 +8699,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -8734,7 +8710,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -8751,7 +8727,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -8768,7 +8744,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -8801,7 +8777,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -8815,7 +8791,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8829,7 +8805,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -8840,7 +8816,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -8851,7 +8827,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -8869,7 +8845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -8881,7 +8857,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -8895,7 +8871,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8909,7 +8885,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -8920,7 +8896,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -8931,7 +8907,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -8961,7 +8937,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -8975,7 +8951,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -8989,7 +8965,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -9000,7 +8976,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -9011,7 +8987,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -9029,7 +9005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -9041,7 +9017,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -9055,7 +9031,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -9069,7 +9045,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -9080,7 +9056,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -9091,7 +9067,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -9109,7 +9085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -9121,7 +9097,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -9135,7 +9111,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -9149,7 +9125,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -9160,7 +9136,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -9171,7 +9147,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -9202,7 +9178,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -9216,7 +9192,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -9230,7 +9206,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -9241,7 +9217,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -9252,7 +9228,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -9282,7 +9258,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -9296,7 +9272,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -9310,7 +9286,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -9321,7 +9297,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -9332,7 +9308,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Modifcation of fr_ca url
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave3.xlsx
+++ b/docs/Language Waves/wave3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="7755" firstSheet="3" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752" firstSheet="7" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="az_az" sheetId="20" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="467">
   <si>
     <t>http://www.cisco.com/web/BG/ordering/index.html</t>
   </si>
@@ -1442,6 +1442,9 @@
   </si>
   <si>
     <t>solutions-listing-var9</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/manufacturing/index_fr.html</t>
   </si>
 </sst>
 </file>
@@ -1975,7 +1978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1989,10 +1992,10 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2065,16 +2068,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:E47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2844,12 +2847,15 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E47"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="65.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>271</v>
       </c>
@@ -2860,7 +2866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>272</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>273</v>
       </c>
@@ -2885,7 +2891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>441</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>274</v>
       </c>
@@ -2907,7 +2913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>275</v>
       </c>
@@ -2921,7 +2927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>276</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>277</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>278</v>
       </c>
@@ -2969,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>279</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>280</v>
       </c>
@@ -3003,7 +3009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>281</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>282</v>
       </c>
@@ -3037,7 +3043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>283</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>284</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>285</v>
       </c>
@@ -3085,7 +3091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>286</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>287</v>
       </c>
@@ -3119,7 +3125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>288</v>
       </c>
@@ -3136,7 +3142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>289</v>
       </c>
@@ -3150,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>290</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>291</v>
       </c>
@@ -3178,7 +3184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>292</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>293</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>294</v>
       </c>
@@ -3229,7 +3235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>295</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>296</v>
       </c>
@@ -3263,7 +3269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>297</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>298</v>
       </c>
@@ -3297,7 +3303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>299</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>300</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>301</v>
       </c>
@@ -3348,7 +3354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>302</v>
       </c>
@@ -3365,7 +3371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>303</v>
       </c>
@@ -3382,7 +3388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>304</v>
       </c>
@@ -3399,7 +3405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>305</v>
       </c>
@@ -3416,7 +3422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>306</v>
       </c>
@@ -3433,7 +3439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>307</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>308</v>
       </c>
@@ -3467,7 +3473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>309</v>
       </c>
@@ -3484,7 +3490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>310</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>311</v>
       </c>
@@ -3518,7 +3524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>312</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>313</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>314</v>
       </c>
@@ -3569,7 +3575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>315</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>316</v>
       </c>
@@ -3619,10 +3625,10 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3750,10 +3756,10 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,11 +3884,11 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4007,11 +4013,11 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4136,10 +4142,10 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4260,13 +4266,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>431</v>
       </c>
@@ -4277,7 +4286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>432</v>
       </c>
@@ -4291,7 +4300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>433</v>
       </c>
@@ -4302,7 +4311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>434</v>
       </c>
@@ -4313,7 +4322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>435</v>
       </c>
@@ -4324,7 +4333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>436</v>
       </c>
@@ -4338,7 +4347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>437</v>
       </c>
@@ -4352,7 +4361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>438</v>
       </c>
@@ -4369,7 +4378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>439</v>
       </c>
@@ -4386,7 +4395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>440</v>
       </c>
@@ -4403,7 +4412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>317</v>
       </c>
@@ -4420,7 +4429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>318</v>
       </c>
@@ -4437,7 +4446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>319</v>
       </c>
@@ -4454,7 +4463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>320</v>
       </c>
@@ -4468,7 +4477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>321</v>
       </c>
@@ -4485,7 +4494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>322</v>
       </c>
@@ -4502,7 +4511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>323</v>
       </c>
@@ -4519,7 +4528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>324</v>
       </c>
@@ -4536,7 +4545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>325</v>
       </c>
@@ -4553,7 +4562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>326</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>327</v>
       </c>
@@ -4581,7 +4590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>328</v>
       </c>
@@ -4595,7 +4604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>329</v>
       </c>
@@ -4612,7 +4621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>330</v>
       </c>
@@ -4629,7 +4638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>331</v>
       </c>
@@ -4646,7 +4655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>332</v>
       </c>
@@ -4663,7 +4672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>333</v>
       </c>
@@ -4680,7 +4689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>334</v>
       </c>
@@ -4697,7 +4706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>335</v>
       </c>
@@ -4714,7 +4723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>336</v>
       </c>
@@ -4731,7 +4740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>337</v>
       </c>
@@ -4748,7 +4757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>338</v>
       </c>
@@ -4765,7 +4774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>339</v>
       </c>
@@ -4782,7 +4791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>340</v>
       </c>
@@ -4799,7 +4808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>341</v>
       </c>
@@ -4816,7 +4825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>342</v>
       </c>
@@ -4833,7 +4842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>343</v>
       </c>
@@ -4850,7 +4859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>344</v>
       </c>
@@ -4867,7 +4876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>345</v>
       </c>
@@ -4884,7 +4893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>346</v>
       </c>
@@ -4901,7 +4910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>347</v>
       </c>
@@ -4918,7 +4927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>348</v>
       </c>
@@ -4935,7 +4944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>349</v>
       </c>
@@ -4952,7 +4961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>350</v>
       </c>
@@ -4969,7 +4978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>351</v>
       </c>
@@ -4986,7 +4995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>352</v>
       </c>
@@ -5003,7 +5012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>353</v>
       </c>
@@ -5033,10 +5042,10 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5161,14 +5170,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5179,7 +5188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -5193,7 +5202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -5215,7 +5224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -5229,7 +5238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -5246,7 +5255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -5263,7 +5272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -5320,10 +5329,10 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5396,19 +5405,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="93.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="93.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -5419,7 +5428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -5433,7 +5442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -5444,7 +5453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -5455,7 +5464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -5466,7 +5475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -5480,7 +5489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -5494,7 +5503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -5511,9 +5520,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>32</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>466</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -5528,7 +5537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -5545,7 +5554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -5562,7 +5571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -5579,7 +5588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -5596,7 +5605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -5613,7 +5622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -5630,7 +5639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -5647,7 +5656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -5664,7 +5673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -5681,7 +5690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -5698,7 +5707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -5715,7 +5724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
@@ -5732,7 +5741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>59</v>
       </c>
@@ -5749,7 +5758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
@@ -5766,7 +5775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
@@ -5783,7 +5792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
@@ -5817,7 +5826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
@@ -5834,7 +5843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
@@ -5851,7 +5860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -5865,7 +5874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>72</v>
       </c>
@@ -5882,7 +5891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>74</v>
       </c>
@@ -5899,7 +5908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>75</v>
       </c>
@@ -5916,7 +5925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
@@ -5933,7 +5942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>80</v>
       </c>
@@ -5950,7 +5959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
@@ -5967,7 +5976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>84</v>
       </c>
@@ -5984,7 +5993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>86</v>
       </c>
@@ -6001,7 +6010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>87</v>
       </c>
@@ -6015,7 +6024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>90</v>
       </c>
@@ -6030,7 +6039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>92</v>
       </c>
@@ -6047,7 +6056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>95</v>
       </c>
@@ -6064,7 +6073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>97</v>
       </c>
@@ -6081,7 +6090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>99</v>
       </c>
@@ -6098,7 +6107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>101</v>
       </c>
@@ -6115,7 +6124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>103</v>
       </c>
@@ -6132,7 +6141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>105</v>
       </c>
@@ -6149,7 +6158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>107</v>
       </c>
@@ -6166,7 +6175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>109</v>
       </c>
@@ -6180,7 +6189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>110</v>
       </c>
@@ -6197,7 +6206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>113</v>
       </c>
@@ -6214,7 +6223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>115</v>
       </c>
@@ -6231,7 +6240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>117</v>
       </c>
@@ -6248,7 +6257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>118</v>
       </c>
@@ -6265,7 +6274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>120</v>
       </c>
@@ -6282,7 +6291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>121</v>
       </c>
@@ -6299,7 +6308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
@@ -6316,7 +6325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>125</v>
       </c>
@@ -6333,7 +6342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>127</v>
       </c>
@@ -6350,7 +6359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
         <v>129</v>
       </c>
@@ -6367,7 +6376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>131</v>
       </c>
@@ -6384,7 +6393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>133</v>
       </c>
@@ -6401,7 +6410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>135</v>
       </c>
@@ -6418,7 +6427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>137</v>
       </c>
@@ -6435,7 +6444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>138</v>
       </c>
@@ -6452,7 +6461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>141</v>
       </c>
@@ -6469,7 +6478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>143</v>
       </c>
@@ -6486,7 +6495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>144</v>
       </c>
@@ -6503,7 +6512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>145</v>
       </c>
@@ -6520,7 +6529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>146</v>
       </c>
@@ -6537,7 +6546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>147</v>
       </c>
@@ -6554,7 +6563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>148</v>
       </c>
@@ -6571,7 +6580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>149</v>
       </c>
@@ -6588,7 +6597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>150</v>
       </c>
@@ -6605,7 +6614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>151</v>
       </c>
@@ -6622,7 +6631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>152</v>
       </c>
@@ -6639,7 +6648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>153</v>
       </c>
@@ -6656,7 +6665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>154</v>
       </c>
@@ -6673,7 +6682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>155</v>
       </c>
@@ -6690,7 +6699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>385</v>
       </c>
@@ -6768,6 +6777,7 @@
     <hyperlink ref="A63" r:id="rId57"/>
     <hyperlink ref="A64" r:id="rId58"/>
     <hyperlink ref="A65" r:id="rId59"/>
+    <hyperlink ref="A9" r:id="rId60"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6777,19 +6787,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>167</v>
       </c>
@@ -6800,7 +6810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>168</v>
       </c>
@@ -6814,7 +6824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>169</v>
       </c>
@@ -6825,7 +6835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>170</v>
       </c>
@@ -6836,7 +6846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>171</v>
       </c>
@@ -6847,7 +6857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>172</v>
       </c>
@@ -6861,7 +6871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>173</v>
       </c>
@@ -6875,7 +6885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>174</v>
       </c>
@@ -6892,7 +6902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -6909,7 +6919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -6926,7 +6936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>176</v>
       </c>
@@ -6943,7 +6953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>177</v>
       </c>
@@ -6960,7 +6970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>178</v>
       </c>
@@ -6977,7 +6987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>179</v>
       </c>
@@ -6994,7 +7004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>180</v>
       </c>
@@ -7011,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>181</v>
       </c>
@@ -7028,7 +7038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>182</v>
       </c>
@@ -7045,7 +7055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>183</v>
       </c>
@@ -7062,7 +7072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>184</v>
       </c>
@@ -7079,7 +7089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>185</v>
       </c>
@@ -7096,7 +7106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>186</v>
       </c>
@@ -7113,7 +7123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>187</v>
       </c>
@@ -7130,7 +7140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>188</v>
       </c>
@@ -7147,7 +7157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>189</v>
       </c>
@@ -7164,7 +7174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>190</v>
       </c>
@@ -7181,7 +7191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>191</v>
       </c>
@@ -7198,7 +7208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>192</v>
       </c>
@@ -7215,7 +7225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>193</v>
       </c>
@@ -7232,7 +7242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>194</v>
       </c>
@@ -7246,7 +7256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>195</v>
       </c>
@@ -7263,7 +7273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>196</v>
       </c>
@@ -7280,7 +7290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>197</v>
       </c>
@@ -7297,7 +7307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>198</v>
       </c>
@@ -7314,7 +7324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>199</v>
       </c>
@@ -7331,7 +7341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>200</v>
       </c>
@@ -7348,7 +7358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>201</v>
       </c>
@@ -7365,7 +7375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>202</v>
       </c>
@@ -7379,7 +7389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>203</v>
       </c>
@@ -7393,7 +7403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>204</v>
       </c>
@@ -7410,7 +7420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>205</v>
       </c>
@@ -7427,7 +7437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>206</v>
       </c>
@@ -7444,7 +7454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>207</v>
       </c>
@@ -7461,7 +7471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>208</v>
       </c>
@@ -7478,7 +7488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>209</v>
       </c>
@@ -7495,7 +7505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>210</v>
       </c>
@@ -7512,7 +7522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>211</v>
       </c>
@@ -7529,7 +7539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>212</v>
       </c>
@@ -7543,7 +7553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>213</v>
       </c>
@@ -7560,7 +7570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>214</v>
       </c>
@@ -7577,7 +7587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>215</v>
       </c>
@@ -7594,7 +7604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>216</v>
       </c>
@@ -7611,7 +7621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>217</v>
       </c>
@@ -7628,7 +7638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>218</v>
       </c>
@@ -7645,7 +7655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>219</v>
       </c>
@@ -7662,7 +7672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>220</v>
       </c>
@@ -7679,7 +7689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>221</v>
       </c>
@@ -7696,7 +7706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>222</v>
       </c>
@@ -7713,7 +7723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
         <v>223</v>
       </c>
@@ -7730,7 +7740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>224</v>
       </c>
@@ -7747,7 +7757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>225</v>
       </c>
@@ -7764,7 +7774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>226</v>
       </c>
@@ -7781,7 +7791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>227</v>
       </c>
@@ -7798,7 +7808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>228</v>
       </c>
@@ -7815,7 +7825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>229</v>
       </c>
@@ -7832,7 +7842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>230</v>
       </c>
@@ -7849,7 +7859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>231</v>
       </c>
@@ -7866,7 +7876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>232</v>
       </c>
@@ -7883,7 +7893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>233</v>
       </c>
@@ -7900,7 +7910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>234</v>
       </c>
@@ -7917,7 +7927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>235</v>
       </c>
@@ -7934,7 +7944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>236</v>
       </c>
@@ -7951,7 +7961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>237</v>
       </c>
@@ -7968,7 +7978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>238</v>
       </c>
@@ -7985,7 +7995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
         <v>239</v>
       </c>
@@ -8002,7 +8012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>240</v>
       </c>
@@ -8019,7 +8029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>241</v>
       </c>
@@ -8036,7 +8046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>242</v>
       </c>
@@ -8053,7 +8063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>382</v>
       </c>
@@ -8070,7 +8080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>383</v>
       </c>
@@ -8105,14 +8115,14 @@
       <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.28515625" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="58.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.109375" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -8249,9 +8259,9 @@
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8376,10 +8386,10 @@
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8504,12 +8514,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8634,11 +8644,11 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8749,10 +8759,10 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8829,10 +8839,10 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8909,10 +8919,10 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8989,10 +8999,10 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9069,10 +9079,10 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9149,11 +9159,11 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9230,10 +9240,10 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>